<commit_message>
diálogos madre y chatarrero
</commit_message>
<xml_diff>
--- a/Assets/Dialogos.xlsx
+++ b/Assets/Dialogos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bohan\GitHub\FUH\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelm\Desktop\FUH\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8544BA1-0D43-43E4-92D7-54EFCCF3124F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EFA4C5-88C4-432B-B99A-D9B711A92712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A325ECA-C1F4-496C-968C-777D88EAB238}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
   <si>
     <t>Role</t>
   </si>
@@ -48,72 +48,18 @@
     <t>Raw Spanish Text</t>
   </si>
   <si>
-    <t>Inicio</t>
-  </si>
-  <si>
     <t>Barry</t>
   </si>
   <si>
     <t>Miranda</t>
   </si>
   <si>
-    <t>Sistema</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
     <t>Chatarero</t>
   </si>
   <si>
-    <t>aaaaaaaaaaaaaaa</t>
-  </si>
-  <si>
-    <t>bbbbbbbbbbbbbbbbbbbbbbb</t>
-  </si>
-  <si>
-    <t>cccccccccccccccccccccccccccccccccc</t>
-  </si>
-  <si>
-    <t>ddddddddddddd</t>
-  </si>
-  <si>
     <t>eeeeeeeeeeeeeeeeeeee</t>
   </si>
   <si>
-    <t>fffffffffffffffffff</t>
-  </si>
-  <si>
-    <t>ggggggggggg</t>
-  </si>
-  <si>
-    <t>hhhhhhhhhhhhhhhhh</t>
-  </si>
-  <si>
-    <t>iiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiiii</t>
-  </si>
-  <si>
     <t>Receptor</t>
   </si>
   <si>
@@ -211,6 +157,57 @@
   </si>
   <si>
     <t>Si lo consigues, llegarás al poblado, ¡buena suerte!</t>
+  </si>
+  <si>
+    <t>Hola hijo, buenos días ¿Dónde estabas?</t>
+  </si>
+  <si>
+    <t>Bueno es igual, necesito que me hagas un favor.</t>
+  </si>
+  <si>
+    <t>Esta nueva enfermedad me está afectando más de lo que esperaba.</t>
+  </si>
+  <si>
+    <t>Por favor, ve a la ferreteria del prueblo a por un poco de  aceite.</t>
+  </si>
+  <si>
+    <t>Muchas gracias hijo.</t>
+  </si>
+  <si>
+    <t>Barry, debes irte de Ferder, el lugar ya no es seguro.</t>
+  </si>
+  <si>
+    <t>Si te vas lejos puede que encuentres a alguien que sepa como ayudarnos.</t>
+  </si>
+  <si>
+    <t>Toma el camino del bosque, quizá el granjero Hamilton te pueda ayudar.</t>
+  </si>
+  <si>
+    <t>La enfermedad nos esta pasando factura a todos, y no hay nadie que nos pueda ayudar.</t>
+  </si>
+  <si>
+    <t>Bienvenido pequeño, ¿Qué necesitas?</t>
+  </si>
+  <si>
+    <t>O vaya, así que un poco de aceite para tu mamá.</t>
+  </si>
+  <si>
+    <t>Espera un segundo, enseguida te lo doy.</t>
+  </si>
+  <si>
+    <t>Espero que esta nueva enfermedad se acabe ya, o esto no afectará a todos.</t>
+  </si>
+  <si>
+    <t>Perfecto, aquí lo tienes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… </t>
+  </si>
+  <si>
+    <t>Miranda1</t>
+  </si>
+  <si>
+    <t>Miranda2</t>
   </si>
 </sst>
 </file>
@@ -590,7 +587,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,13 +602,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -622,7 +619,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -631,18 +628,18 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -651,18 +648,18 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -671,18 +668,18 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -691,18 +688,18 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -711,18 +708,18 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -731,18 +728,18 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -751,18 +748,18 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -771,179 +768,179 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
         <v>4</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -952,18 +949,18 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -972,18 +969,18 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -992,18 +989,18 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1012,18 +1009,18 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1032,18 +1029,18 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1052,18 +1049,18 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1072,18 +1069,18 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1092,18 +1089,18 @@
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1112,18 +1109,18 @@
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1132,18 +1129,18 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1152,18 +1149,18 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1172,18 +1169,18 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1192,18 +1189,18 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1212,18 +1209,18 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1232,18 +1229,18 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1252,18 +1249,18 @@
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1272,13 +1269,13 @@
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>